<commit_message>
Grid parallel execution code with showing reports parallely
</commit_message>
<xml_diff>
--- a/data/ImageSubPortal.xlsx
+++ b/data/ImageSubPortal.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\ESRI_TEST\com.esri.test.automation\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="141"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="6450" tabRatio="141"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>pagetitle</t>
   </si>
@@ -42,30 +37,49 @@
     <t>rblbl2</t>
   </si>
   <si>
-    <t>Upload Your Images</t>
-  </si>
-  <si>
-    <t>For which conference are you submitting images?</t>
-  </si>
-  <si>
     <t>Non-specific Events (Dec 31 2016)</t>
   </si>
   <si>
-    <t>What type of files are you submitting?</t>
-  </si>
-  <si>
     <t>Are you a Federal Government Employee?</t>
+  </si>
+  <si>
+    <t>Upload Your Images</t>
+  </si>
+  <si>
+    <t>For which conference are you submitting images?</t>
+  </si>
+  <si>
+    <t>p2Title</t>
+  </si>
+  <si>
+    <t>Copyright Permission and Release Form</t>
+  </si>
+  <si>
+    <t>p3Title</t>
+  </si>
+  <si>
+    <t>Do any of the images include identifiable people?</t>
+  </si>
+  <si>
+    <t>What type of files are you submitting?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,14 +99,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -150,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -185,7 +203,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -362,7 +380,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -373,18 +391,23 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125"/>
+    <col min="1" max="3" width="11.5703125"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.5703125"/>
+    <col min="8" max="8" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,25 +426,37 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Framework with sample code
</commit_message>
<xml_diff>
--- a/data/ImageSubPortal.xlsx
+++ b/data/ImageSubPortal.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\ESRI_TEST\com.esri.test.automation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working_on_LT\com.esri.test.automation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="141"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="6450" tabRatio="141"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>pagetitle</t>
   </si>
@@ -42,30 +42,56 @@
     <t>rblbl2</t>
   </si>
   <si>
-    <t>Upload Your Images</t>
-  </si>
-  <si>
-    <t>For which conference are you submitting images?</t>
-  </si>
-  <si>
     <t>Non-specific Events (Dec 31 2016)</t>
   </si>
   <si>
-    <t>What type of files are you submitting?</t>
-  </si>
-  <si>
-    <t>Are you a Federal Government Employee?</t>
+    <t>Upload Your Images</t>
+  </si>
+  <si>
+    <t>For which conference are you submitting images?</t>
+  </si>
+  <si>
+    <t>p2Title</t>
+  </si>
+  <si>
+    <t>p3Title</t>
+  </si>
+  <si>
+    <t>What type of files are you submitting?</t>
+  </si>
+  <si>
+    <t>Are you a Federal Government Employee?</t>
+  </si>
+  <si>
+    <t>Copyright Permission and Release Form</t>
+  </si>
+  <si>
+    <t>Do any of the images include identifiable people?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,14 +111,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -373,18 +404,24 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125"/>
+    <col min="1" max="2" width="11.5703125"/>
+    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125"/>
+    <col min="7" max="7" width="45.28515625" customWidth="1"/>
+    <col min="8" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,25 +440,37 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
uploading the changed wrappers methods and sites
</commit_message>
<xml_diff>
--- a/data/ImageSubPortal.xlsx
+++ b/data/ImageSubPortal.xlsx
@@ -3,23 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Working_on_LT\com.esri.test.automation\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="6450" tabRatio="141"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="4845" tabRatio="141"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>pagetitle</t>
   </si>
@@ -67,13 +63,19 @@
   </si>
   <si>
     <t>Do any of the images include identifiable people?</t>
+  </si>
+  <si>
+    <t>ISPUrl</t>
+  </si>
+  <si>
+    <t>http://www.esri.com/events/image-submissions#/home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -93,6 +95,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -111,17 +120,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -404,78 +416,87 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.5703125"/>
-    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125"/>
-    <col min="7" max="7" width="45.28515625" customWidth="1"/>
-    <col min="8" max="1025" width="11.5703125"/>
+    <col min="2" max="3" width="11.5703125"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125"/>
+    <col min="8" max="8" width="45.28515625" customWidth="1"/>
+    <col min="9" max="1026" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" location="/home"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>